<commit_message>
Working on concept model 4: working with all constraints (child-parent vars).
</commit_message>
<xml_diff>
--- a/default/4_sut_multi_year_rcot_cap_new/concept.xlsx
+++ b/default/4_sut_multi_year_rcot_cap_new/concept.xlsx
@@ -5,15 +5,15 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\loren\Documents\GitHub\pyesm\default\3_sut_multi_year_rcot_cap\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git_repos\pyesm\default\4_sut_multi_year_rcot_cap_new\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57740533-B7D6-4DD6-8D33-135559005B6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2F08D0A-C0F3-4CA2-BCBB-F39C943C5779}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-38510" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="no disposal" sheetId="2" r:id="rId1"/>
+    <sheet name="no disposal" sheetId="6" r:id="rId1"/>
     <sheet name="disposal_mat" sheetId="3" r:id="rId2"/>
     <sheet name="disposal" sheetId="4" r:id="rId3"/>
     <sheet name="discounting" sheetId="5" r:id="rId4"/>
@@ -22,7 +22,7 @@
     <definedName name="OpenSolver_ChosenSolver" localSheetId="3" hidden="1">CBC</definedName>
     <definedName name="OpenSolver_ChosenSolver" localSheetId="2" hidden="1">CBC</definedName>
     <definedName name="OpenSolver_ChosenSolver" localSheetId="1" hidden="1">CBC</definedName>
-    <definedName name="OpenSolver_ChosenSolver" localSheetId="0" hidden="1">CBC</definedName>
+    <definedName name="OpenSolver_ChosenSolver" localSheetId="0" hidden="1">Gurobi</definedName>
     <definedName name="OpenSolver_DualsNewSheet" localSheetId="3" hidden="1">0</definedName>
     <definedName name="OpenSolver_DualsNewSheet" localSheetId="2" hidden="1">0</definedName>
     <definedName name="OpenSolver_DualsNewSheet" localSheetId="1" hidden="1">0</definedName>
@@ -38,7 +38,7 @@
     <definedName name="solver_adj" localSheetId="3" hidden="1">discounting!$F$27:$H$31,discounting!$N$27:$P$31,discounting!$J$27:$L$31</definedName>
     <definedName name="solver_adj" localSheetId="2" hidden="1">disposal!$F$27:$H$31,disposal!$N$27:$P$31,disposal!$J$27:$L$31</definedName>
     <definedName name="solver_adj" localSheetId="1" hidden="1">disposal_mat!$F$27:$H$31,disposal_mat!$N$27:$P$31,disposal_mat!$J$27:$L$31</definedName>
-    <definedName name="solver_adj" localSheetId="0" hidden="1">'no disposal'!$F$24:$H$28,'no disposal'!$N$24:$P$28,'no disposal'!$J$24:$L$28</definedName>
+    <definedName name="solver_adj" localSheetId="0" hidden="1">'no disposal'!$F$24:$H$28,'no disposal'!$J$24:$L$28,'no disposal'!$N$24:$P$28</definedName>
     <definedName name="solver_cvg" localSheetId="3" hidden="1">0.0001</definedName>
     <definedName name="solver_cvg" localSheetId="2" hidden="1">0.0001</definedName>
     <definedName name="solver_cvg" localSheetId="1" hidden="1">0.0001</definedName>
@@ -66,7 +66,7 @@
     <definedName name="solver_lhs2" localSheetId="3" hidden="1">discounting!$F$27:$H$31</definedName>
     <definedName name="solver_lhs2" localSheetId="2" hidden="1">disposal!$F$27:$H$31</definedName>
     <definedName name="solver_lhs2" localSheetId="1" hidden="1">disposal_mat!$F$27:$H$31</definedName>
-    <definedName name="solver_lhs2" localSheetId="0" hidden="1">'no disposal'!$F$24:$H$28</definedName>
+    <definedName name="solver_lhs2" localSheetId="0" hidden="1">'no disposal'!$Z$7:$AD$8</definedName>
     <definedName name="solver_lhs3" localSheetId="3" hidden="1">discounting!$J$27:$L$31</definedName>
     <definedName name="solver_lhs3" localSheetId="2" hidden="1">disposal!$J$27:$L$31</definedName>
     <definedName name="solver_lhs3" localSheetId="1" hidden="1">disposal_mat!$J$27:$L$31</definedName>
@@ -74,7 +74,7 @@
     <definedName name="solver_lhs4" localSheetId="3" hidden="1">discounting!$J$34:$L$38</definedName>
     <definedName name="solver_lhs4" localSheetId="2" hidden="1">disposal!$J$34:$L$38</definedName>
     <definedName name="solver_lhs4" localSheetId="1" hidden="1">disposal_mat!$J$34:$L$38</definedName>
-    <definedName name="solver_lhs4" localSheetId="0" hidden="1">'no disposal'!$J$32:$L$36</definedName>
+    <definedName name="solver_lhs4" localSheetId="0" hidden="1">'no disposal'!$J$24:$L$28</definedName>
     <definedName name="solver_lhs5" localSheetId="3" hidden="1">discounting!$Z$7:$AD$8</definedName>
     <definedName name="solver_lhs5" localSheetId="2" hidden="1">disposal!$Z$7:$AD$8</definedName>
     <definedName name="solver_lhs5" localSheetId="1" hidden="1">disposal_mat!$AD$7:$AH$8</definedName>
@@ -110,7 +110,7 @@
     <definedName name="solver_num" localSheetId="3" hidden="1">5</definedName>
     <definedName name="solver_num" localSheetId="2" hidden="1">5</definedName>
     <definedName name="solver_num" localSheetId="1" hidden="1">5</definedName>
-    <definedName name="solver_num" localSheetId="0" hidden="1">5</definedName>
+    <definedName name="solver_num" localSheetId="0" hidden="1">4</definedName>
     <definedName name="solver_nwt" localSheetId="3" hidden="1">1</definedName>
     <definedName name="solver_nwt" localSheetId="2" hidden="1">1</definedName>
     <definedName name="solver_nwt" localSheetId="1" hidden="1">1</definedName>
@@ -134,7 +134,7 @@
     <definedName name="solver_rel2" localSheetId="3" hidden="1">3</definedName>
     <definedName name="solver_rel2" localSheetId="2" hidden="1">3</definedName>
     <definedName name="solver_rel2" localSheetId="1" hidden="1">3</definedName>
-    <definedName name="solver_rel2" localSheetId="0" hidden="1">3</definedName>
+    <definedName name="solver_rel2" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_rel3" localSheetId="3" hidden="1">1</definedName>
     <definedName name="solver_rel3" localSheetId="2" hidden="1">1</definedName>
     <definedName name="solver_rel3" localSheetId="1" hidden="1">1</definedName>
@@ -142,7 +142,7 @@
     <definedName name="solver_rel4" localSheetId="3" hidden="1">1</definedName>
     <definedName name="solver_rel4" localSheetId="2" hidden="1">1</definedName>
     <definedName name="solver_rel4" localSheetId="1" hidden="1">1</definedName>
-    <definedName name="solver_rel4" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_rel4" localSheetId="0" hidden="1">3</definedName>
     <definedName name="solver_rel5" localSheetId="3" hidden="1">2</definedName>
     <definedName name="solver_rel5" localSheetId="2" hidden="1">2</definedName>
     <definedName name="solver_rel5" localSheetId="1" hidden="1">2</definedName>
@@ -166,7 +166,7 @@
     <definedName name="solver_rhs4" localSheetId="3" hidden="1">discounting!$J$27:$L$31</definedName>
     <definedName name="solver_rhs4" localSheetId="2" hidden="1">disposal!$J$27:$L$31</definedName>
     <definedName name="solver_rhs4" localSheetId="1" hidden="1">disposal_mat!$J$27:$L$31</definedName>
-    <definedName name="solver_rhs4" localSheetId="0" hidden="1">'no disposal'!$J$24:$L$28</definedName>
+    <definedName name="solver_rhs4" localSheetId="0" hidden="1">'no disposal'!$J$32:$L$36</definedName>
     <definedName name="solver_rhs5" localSheetId="3" hidden="1">0</definedName>
     <definedName name="solver_rhs5" localSheetId="2" hidden="1">0</definedName>
     <definedName name="solver_rhs5" localSheetId="1" hidden="1">0</definedName>
@@ -592,11 +592,12 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0E+00"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
+    <numFmt numFmtId="167" formatCode="0.0"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -607,12 +608,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -746,7 +741,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment textRotation="90" wrapText="1"/>
@@ -763,8 +758,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
@@ -773,19 +768,30 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="1" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -801,6 +807,1211 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="170" name="OpenSolver1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{72664EAA-9477-5AA6-EFC8-E37AC5180C85}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4184650" y="5257800"/>
+          <a:ext cx="1543050" cy="920750"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FF00FF">
+            <a:alpha val="40000"/>
+          </a:srgbClr>
+        </a:solidFill>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:noFill/>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:effectLst/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" lIns="25400" tIns="25400" rIns="0" bIns="0" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="it-IT" sz="1100" b="1">
+            <a:solidFill>
+              <a:srgbClr val="FF00FF"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="171" name="OpenSolver2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{32EB2C87-F612-4AA1-3095-3D815789AD85}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6242050" y="5257800"/>
+          <a:ext cx="1543050" cy="920750"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FF00FF">
+            <a:alpha val="40000"/>
+          </a:srgbClr>
+        </a:solidFill>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:noFill/>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:effectLst/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" lIns="25400" tIns="25400" rIns="0" bIns="0" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="it-IT" sz="1100" b="1">
+            <a:solidFill>
+              <a:srgbClr val="FF00FF"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="172" name="OpenSolver3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7E950FE5-69DD-98D6-060D-43C74B835DA3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8299450" y="5257800"/>
+          <a:ext cx="1543050" cy="920750"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FF00FF">
+            <a:alpha val="40000"/>
+          </a:srgbClr>
+        </a:solidFill>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:noFill/>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:effectLst/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" lIns="25400" tIns="25400" rIns="0" bIns="0" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="it-IT" sz="1100" b="1">
+            <a:solidFill>
+              <a:srgbClr val="FF00FF"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="173" name="OpenSolver4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A53FB7A3-DA81-763A-BB3D-DADDE66214CA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11385550" y="3416300"/>
+          <a:ext cx="514350" cy="184150"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:srgbClr val="FF00FF"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:effectLst/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" lIns="25400" tIns="25400" rIns="0" bIns="0" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="it-IT" sz="1100" b="1">
+            <a:solidFill>
+              <a:srgbClr val="FF00FF"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>508000</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>107950</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>224739</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="174" name="OpenSolver5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D2D06670-0E11-250E-A434-46D5A87A09C4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11379200" y="3340100"/>
+          <a:ext cx="231089" cy="127000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF">
+            <a:alpha val="80000"/>
+          </a:srgbClr>
+        </a:solidFill>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:noFill/>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:effectLst/>
+        <a:extLst>
+          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="12700" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:shade val="15000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:prstDash val="solid"/>
+              <a:miter lim="800000"/>
+            </a14:hiddenLine>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" lIns="12700" tIns="0" rIns="12700" bIns="0" rtlCol="0" anchor="t">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="it-IT" sz="900">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>min </a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="175" name="OpenSolverZ10:AD12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BC19E383-3CE3-0925-27E6-22654F8AABA8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="14471650" y="2679700"/>
+          <a:ext cx="2571750" cy="552450"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:srgbClr val="0000FF"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:effectLst/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" lIns="25400" tIns="25400" rIns="0" bIns="0" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="it-IT" sz="1100" b="1">
+              <a:solidFill>
+                <a:srgbClr val="0000FF"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>0=</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="176" name="OpenSolverZ7:AD8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F67C62C5-6236-BE63-35F7-F3D0D462B8B2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="14471650" y="2127250"/>
+          <a:ext cx="2571750" cy="368300"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:srgbClr val="008000"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:effectLst/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" lIns="25400" tIns="25400" rIns="0" bIns="0" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="it-IT" sz="1100" b="1">
+              <a:solidFill>
+                <a:srgbClr val="008000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>0=</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>12700</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="177" name="OpenSolver8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EE891B1C-3D26-5C66-A86A-7AB7678D2608}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6254750" y="5270500"/>
+          <a:ext cx="1530350" cy="908050"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:srgbClr val="9900CC"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:effectLst/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" lIns="25400" tIns="25400" rIns="0" bIns="0" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="it-IT" sz="1100" b="1">
+            <a:solidFill>
+              <a:srgbClr val="9900CC"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="178" name="OpenSolver9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{86E042BE-1F9A-AFC2-A6CB-35F226E2BF38}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6242050" y="8020050"/>
+          <a:ext cx="1543050" cy="920750"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:srgbClr val="9900CC"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:effectLst/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" lIns="25400" tIns="25400" rIns="0" bIns="0" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="it-IT" sz="1100" b="1">
+              <a:solidFill>
+                <a:srgbClr val="9900CC"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>≤</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>257175</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>263525</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="179" name="OpenSolver10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7BAA50D7-3B51-E5C6-04EC-CC8144A29436}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="177" idx="2"/>
+          <a:endCxn id="178" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="7013575" y="6178550"/>
+          <a:ext cx="6350" cy="1841500"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:srgbClr val="9900CC"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:headEnd type="none"/>
+          <a:tailEnd type="none"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>69850</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>450850</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="180" name="OpenSolver11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{80DCB820-55DB-8FB4-23CB-174408464998}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6826250" y="6972300"/>
+          <a:ext cx="381000" cy="254000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:noFill/>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:effectLst/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="12700" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:shade val="15000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:prstDash val="solid"/>
+              <a:miter lim="800000"/>
+            </a14:hiddenLine>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="it-IT" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>25400</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="181" name="OpenSolver12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EBBF5B4C-885F-B4E4-2B4F-3102FAC3BF63}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6267450" y="5283200"/>
+          <a:ext cx="1517650" cy="895350"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:srgbClr val="800000"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:effectLst/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" lIns="25400" tIns="25400" rIns="0" bIns="0" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="it-IT" sz="1100" b="1">
+            <a:solidFill>
+              <a:srgbClr val="800000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="182" name="OpenSolver13">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{85FB9B45-3CA1-FB66-46CD-B2DFACA86355}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6242050" y="6731000"/>
+          <a:ext cx="1543050" cy="920750"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:srgbClr val="800000"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:effectLst/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" lIns="25400" tIns="25400" rIns="0" bIns="0" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="it-IT" sz="1100" b="1">
+              <a:solidFill>
+                <a:srgbClr val="800000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>≥</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>257175</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>269875</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="183" name="OpenSolver14">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B73E8506-C25C-6D85-B2D6-5AA212C6CBF4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="181" idx="2"/>
+          <a:endCxn id="182" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="7013575" y="6178550"/>
+          <a:ext cx="12700" cy="552450"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:srgbClr val="800000"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:headEnd type="none"/>
+          <a:tailEnd type="none"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>73025</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>149225</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>454025</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>34925</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="184" name="OpenSolver15">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F72E6C86-A0DE-FE12-1B23-A94F103A340F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6829425" y="6327775"/>
+          <a:ext cx="381000" cy="254000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:noFill/>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:effectLst/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="12700" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:shade val="15000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:prstDash val="solid"/>
+              <a:miter lim="800000"/>
+            </a14:hiddenLine>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="it-IT" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1065,31 +2276,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43994AB8-4797-4F82-A05D-BD00A3481ACB}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DEA8235-8641-4C81-8A66-786129DBD094}">
   <dimension ref="A1:AH50"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="5" ySplit="6" topLeftCell="F7" activePane="bottomRight" state="frozen"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane xSplit="5" ySplit="6" topLeftCell="F16" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="N32" sqref="N32"/>
+      <selection pane="bottomRight" activeCell="Z38" sqref="Z38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="4" max="4" width="23.453125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.26953125" bestFit="1" customWidth="1"/>
-    <col min="6" max="8" width="6.453125" customWidth="1"/>
-    <col min="9" max="9" width="4.7265625" customWidth="1"/>
-    <col min="10" max="12" width="6.81640625" customWidth="1"/>
-    <col min="13" max="13" width="4.7265625" customWidth="1"/>
-    <col min="14" max="16" width="7.453125" customWidth="1"/>
-    <col min="17" max="18" width="6.26953125" customWidth="1"/>
-    <col min="19" max="19" width="4.81640625" customWidth="1"/>
-    <col min="20" max="30" width="7.453125" customWidth="1"/>
-    <col min="31" max="32" width="4.81640625" customWidth="1"/>
-    <col min="33" max="33" width="5.26953125" customWidth="1"/>
-    <col min="34" max="36" width="7.1796875" customWidth="1"/>
+    <col min="6" max="34" width="7.36328125" customWidth="1"/>
+    <col min="35" max="36" width="7.1796875" customWidth="1"/>
     <col min="37" max="41" width="5.26953125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1232,52 +2434,52 @@
       <c r="L7" s="2">
         <v>0</v>
       </c>
-      <c r="N7" s="3">
+      <c r="N7" s="31">
         <v>100</v>
       </c>
-      <c r="O7" s="3">
+      <c r="O7" s="31">
         <v>120</v>
       </c>
-      <c r="P7" s="3">
+      <c r="P7" s="31">
         <v>144</v>
       </c>
-      <c r="Q7" s="3">
+      <c r="Q7" s="31">
         <v>173</v>
       </c>
-      <c r="R7" s="3">
+      <c r="R7" s="31">
         <v>207</v>
       </c>
-      <c r="T7">
+      <c r="T7" s="33">
         <f t="array" ref="T7:X8">MMULT(AF7:AH8,TRANSPOSE(F24:H28))</f>
-        <v>108.57763</v>
-      </c>
-      <c r="U7">
-        <v>130.29316</v>
-      </c>
-      <c r="V7">
-        <v>156.35178999999999</v>
-      </c>
-      <c r="W7">
-        <v>187.83931000000001</v>
-      </c>
-      <c r="X7">
-        <v>224.75569999999999</v>
-      </c>
-      <c r="Z7" s="13">
+        <v>108.57763300759967</v>
+      </c>
+      <c r="U7" s="33">
+        <v>130.29315960911961</v>
+      </c>
+      <c r="V7" s="33">
+        <v>156.35179153094353</v>
+      </c>
+      <c r="W7" s="33">
+        <v>187.83930510314454</v>
+      </c>
+      <c r="X7" s="33">
+        <v>224.75570032572784</v>
+      </c>
+      <c r="Z7" s="34">
         <f t="array" ref="Z7:AD8">T7:X8-MMULT(J7:L8,TRANSPOSE(J24:L28))-N7:R8</f>
-        <v>-2.7699999947117249E-6</v>
-      </c>
-      <c r="AA7" s="6">
-        <v>3.6000000136482413E-7</v>
-      </c>
-      <c r="AB7" s="6">
-        <v>-1.4100000100825127E-6</v>
-      </c>
-      <c r="AC7" s="6">
-        <v>4.5099999965714233E-6</v>
-      </c>
-      <c r="AD7" s="7">
-        <v>-3.0000001061125658E-7</v>
+        <v>-6.9633188104489818E-13</v>
+      </c>
+      <c r="AA7" s="35">
+        <v>-8.3844042819691822E-13</v>
+      </c>
+      <c r="AB7" s="35">
+        <v>-1.0231815394945443E-12</v>
+      </c>
+      <c r="AC7" s="35">
+        <v>-3.865352482534945E-12</v>
+      </c>
+      <c r="AD7" s="36">
+        <v>-4.6611603465862572E-12</v>
       </c>
       <c r="AF7" s="2">
         <v>1</v>
@@ -1308,50 +2510,50 @@
       <c r="L8" s="2">
         <v>0</v>
       </c>
-      <c r="N8" s="3">
+      <c r="N8" s="31">
         <v>508022.19999999995</v>
       </c>
-      <c r="O8" s="3">
+      <c r="O8" s="31">
         <v>518182.64399999997</v>
       </c>
-      <c r="P8" s="3">
+      <c r="P8" s="31">
         <v>528546.29687999992</v>
       </c>
-      <c r="Q8" s="3">
+      <c r="Q8" s="31">
         <v>539117.22281759989</v>
       </c>
-      <c r="R8" s="3">
+      <c r="R8" s="31">
         <v>549899.56727395195</v>
       </c>
-      <c r="T8">
+      <c r="T8" s="33">
         <v>508022.2</v>
       </c>
-      <c r="U8">
-        <v>518182.64</v>
-      </c>
-      <c r="V8">
-        <v>528546.30000000005</v>
-      </c>
-      <c r="W8">
-        <v>539117.22</v>
-      </c>
-      <c r="X8">
-        <v>549899.56999999995</v>
-      </c>
-      <c r="Z8" s="8">
-        <v>0</v>
-      </c>
-      <c r="AA8" s="9">
-        <v>-3.9999999571591616E-3</v>
-      </c>
-      <c r="AB8" s="9">
-        <v>3.1200001249089837E-3</v>
-      </c>
-      <c r="AC8" s="9">
-        <v>-2.8175999177619815E-3</v>
-      </c>
-      <c r="AD8" s="10">
-        <v>2.7260479982942343E-3</v>
+      <c r="U8" s="33">
+        <v>518182.64399999997</v>
+      </c>
+      <c r="V8" s="33">
+        <v>528546.29688000004</v>
+      </c>
+      <c r="W8" s="33">
+        <v>539117.22281760001</v>
+      </c>
+      <c r="X8" s="33">
+        <v>549899.56727395195</v>
+      </c>
+      <c r="Z8" s="37">
+        <v>0</v>
+      </c>
+      <c r="AA8" s="38">
+        <v>0</v>
+      </c>
+      <c r="AB8" s="38">
+        <v>0</v>
+      </c>
+      <c r="AC8" s="38">
+        <v>0</v>
+      </c>
+      <c r="AD8" s="39">
+        <v>0</v>
       </c>
       <c r="AF8" s="2">
         <v>0</v>
@@ -1395,20 +2597,20 @@
       <c r="V10" s="4"/>
       <c r="W10" s="4"/>
       <c r="X10" s="4"/>
-      <c r="Z10" s="5">
+      <c r="Z10" s="34">
         <f t="array" ref="Z10:AD12">TRANSPOSE(J24:L28)-MMULT(F10:H12,TRANSPOSE(F24:H28))</f>
         <v>0</v>
       </c>
-      <c r="AA10" s="6">
-        <v>0</v>
-      </c>
-      <c r="AB10" s="6">
-        <v>0</v>
-      </c>
-      <c r="AC10" s="6">
-        <v>0</v>
-      </c>
-      <c r="AD10" s="7">
+      <c r="AA10" s="35">
+        <v>0</v>
+      </c>
+      <c r="AB10" s="35">
+        <v>0</v>
+      </c>
+      <c r="AC10" s="35">
+        <v>0</v>
+      </c>
+      <c r="AD10" s="36">
         <v>0</v>
       </c>
     </row>
@@ -1436,19 +2638,19 @@
       <c r="V11" s="4"/>
       <c r="W11" s="4"/>
       <c r="X11" s="4"/>
-      <c r="Z11" s="11">
-        <v>0</v>
-      </c>
-      <c r="AA11">
-        <v>0</v>
-      </c>
-      <c r="AB11">
-        <v>0</v>
-      </c>
-      <c r="AC11">
-        <v>0</v>
-      </c>
-      <c r="AD11" s="12">
+      <c r="Z11" s="40">
+        <v>0</v>
+      </c>
+      <c r="AA11" s="32">
+        <v>0</v>
+      </c>
+      <c r="AB11" s="32">
+        <v>0</v>
+      </c>
+      <c r="AC11" s="32">
+        <v>0</v>
+      </c>
+      <c r="AD11" s="41">
         <v>0</v>
       </c>
     </row>
@@ -1476,19 +2678,19 @@
       <c r="V12" s="4"/>
       <c r="W12" s="4"/>
       <c r="X12" s="4"/>
-      <c r="Z12" s="8">
-        <v>0</v>
-      </c>
-      <c r="AA12" s="9">
-        <v>0</v>
-      </c>
-      <c r="AB12" s="9">
-        <v>0</v>
-      </c>
-      <c r="AC12" s="9">
-        <v>0</v>
-      </c>
-      <c r="AD12" s="10">
+      <c r="Z12" s="37">
+        <v>0</v>
+      </c>
+      <c r="AA12" s="38">
+        <v>0</v>
+      </c>
+      <c r="AB12" s="38">
+        <v>0</v>
+      </c>
+      <c r="AC12" s="38">
+        <v>0</v>
+      </c>
+      <c r="AD12" s="39">
         <v>0</v>
       </c>
     </row>
@@ -1511,7 +2713,7 @@
         <v>10</v>
       </c>
       <c r="K14" s="2">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="L14" s="2">
         <v>5</v>
@@ -1520,8 +2722,8 @@
         <v>55</v>
       </c>
       <c r="T14" s="15">
-        <f>SUM(R24:T28,R32:T36)</f>
-        <v>2651862.165910033</v>
+        <f>SUM(R32:T36)+SUM(R24:T28)</f>
+        <v>2643770.7831718032</v>
       </c>
     </row>
     <row r="15" spans="1:34" x14ac:dyDescent="0.35">
@@ -1538,7 +2740,7 @@
         <v>10</v>
       </c>
       <c r="K15" s="2">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="L15" s="2">
         <v>1</v>
@@ -1598,7 +2800,7 @@
         <v>0.3</v>
       </c>
       <c r="L18" s="2">
-        <v>20</v>
+        <v>200</v>
       </c>
     </row>
     <row r="19" spans="1:20" x14ac:dyDescent="0.35">
@@ -1679,41 +2881,41 @@
         <v>24</v>
       </c>
       <c r="F24" s="16">
-        <v>108.57763</v>
+        <v>0</v>
       </c>
       <c r="G24" s="17">
-        <v>0</v>
+        <v>108.57763300759967</v>
       </c>
       <c r="H24" s="18">
         <v>508022.2</v>
       </c>
       <c r="J24" s="16">
-        <v>108.57763</v>
+        <v>0</v>
       </c>
       <c r="K24" s="17">
-        <v>0</v>
+        <v>108.57763300759967</v>
       </c>
       <c r="L24" s="18">
         <v>508022.2</v>
       </c>
       <c r="N24" s="16">
-        <v>1.7706724E-2</v>
+        <v>0</v>
       </c>
       <c r="O24" s="17">
-        <v>0</v>
+        <v>8.552347805392993E-2</v>
       </c>
       <c r="P24" s="18">
-        <v>2.8996700999999998</v>
+        <v>0.28996700913242007</v>
       </c>
       <c r="R24">
         <f t="array" ref="R24:T28">MMULT(N24:P28,_xlfn.MUNIT(3)*J14:L14)</f>
-        <v>0.17706724000000001</v>
+        <v>0</v>
       </c>
       <c r="S24">
-        <v>0</v>
+        <v>1.2828521708089489</v>
       </c>
       <c r="T24">
-        <v>14.498350499999999</v>
+        <v>1.4498350456621003</v>
       </c>
     </row>
     <row r="25" spans="1:20" x14ac:dyDescent="0.35">
@@ -1721,40 +2923,40 @@
         <v>25</v>
       </c>
       <c r="F25" s="19">
-        <v>130.29316</v>
+        <v>0</v>
       </c>
       <c r="G25" s="4">
-        <v>0</v>
+        <v>130.29315960911961</v>
       </c>
       <c r="H25" s="20">
-        <v>518182.64</v>
+        <v>518182.64399999997</v>
       </c>
       <c r="J25" s="19">
-        <v>130.29316</v>
+        <v>0</v>
       </c>
       <c r="K25" s="4">
-        <v>0</v>
+        <v>130.29315960911961</v>
       </c>
       <c r="L25" s="20">
-        <v>518182.64</v>
+        <v>518182.64399999997</v>
       </c>
       <c r="N25" s="19">
-        <v>3.5413447999999999E-3</v>
+        <v>0</v>
       </c>
       <c r="O25" s="4">
         <v>0</v>
       </c>
       <c r="P25" s="20">
-        <v>5.7993401999999999E-2</v>
+        <v>5.7993401826483791E-3</v>
       </c>
       <c r="R25">
-        <v>3.5413448E-2</v>
+        <v>0</v>
       </c>
       <c r="S25">
         <v>0</v>
       </c>
       <c r="T25">
-        <v>0.28996701000000003</v>
+        <v>2.8996700913241896E-2</v>
       </c>
     </row>
     <row r="26" spans="1:20" x14ac:dyDescent="0.35">
@@ -1762,40 +2964,40 @@
         <v>26</v>
       </c>
       <c r="F26" s="19">
-        <v>156.35178999999999</v>
+        <v>0</v>
       </c>
       <c r="G26" s="4">
-        <v>0</v>
+        <v>156.35179153094353</v>
       </c>
       <c r="H26" s="20">
-        <v>528546.30000000005</v>
+        <v>528546.29688000004</v>
       </c>
       <c r="J26" s="19">
-        <v>156.35178999999999</v>
+        <v>0</v>
       </c>
       <c r="K26" s="4">
-        <v>0</v>
+        <v>156.35179153094353</v>
       </c>
       <c r="L26" s="20">
-        <v>528546.30000000005</v>
+        <v>528546.29688000004</v>
       </c>
       <c r="N26" s="19">
-        <v>4.2496137999999996E-3</v>
+        <v>0</v>
       </c>
       <c r="O26" s="4">
         <v>0</v>
       </c>
       <c r="P26" s="20">
-        <v>5.9153270000000001E-2</v>
+        <v>1.81032667088767E-2</v>
       </c>
       <c r="R26">
-        <v>4.2496137999999996E-2</v>
+        <v>0</v>
       </c>
       <c r="S26">
         <v>0</v>
       </c>
       <c r="T26">
-        <v>0.29576635000000001</v>
+        <v>9.0516333544383501E-2</v>
       </c>
     </row>
     <row r="27" spans="1:20" x14ac:dyDescent="0.35">
@@ -1803,40 +3005,40 @@
         <v>27</v>
       </c>
       <c r="F27" s="19">
-        <v>187.83931000000001</v>
+        <v>0</v>
       </c>
       <c r="G27" s="4">
-        <v>0</v>
+        <v>187.83930510314454</v>
       </c>
       <c r="H27" s="20">
-        <v>539117.22</v>
+        <v>539117.22281760001</v>
       </c>
       <c r="J27" s="19">
-        <v>187.83931000000001</v>
+        <v>0</v>
       </c>
       <c r="K27" s="4">
-        <v>0</v>
+        <v>187.83930510314454</v>
       </c>
       <c r="L27" s="20">
-        <v>539117.22</v>
+        <v>539117.22281760001</v>
       </c>
       <c r="N27" s="19">
-        <v>5.1349500000000001E-3</v>
+        <v>0</v>
       </c>
       <c r="O27" s="4">
         <v>0</v>
       </c>
       <c r="P27" s="20">
-        <v>6.0336334999999998E-2</v>
+        <v>0</v>
       </c>
       <c r="R27">
-        <v>5.1349499999999999E-2</v>
+        <v>0</v>
       </c>
       <c r="S27">
         <v>0</v>
       </c>
       <c r="T27">
-        <v>0.30168167499999998</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:20" x14ac:dyDescent="0.35">
@@ -1844,40 +3046,40 @@
         <v>28</v>
       </c>
       <c r="F28" s="21">
-        <v>224.75569999999999</v>
+        <v>0</v>
       </c>
       <c r="G28" s="22">
-        <v>0</v>
+        <v>224.75570032572784</v>
       </c>
       <c r="H28" s="23">
-        <v>549899.56999999995</v>
+        <v>549899.56727395195</v>
       </c>
       <c r="J28" s="21">
-        <v>224.75569999999999</v>
+        <v>0</v>
       </c>
       <c r="K28" s="22">
-        <v>0</v>
+        <v>224.75570032572784</v>
       </c>
       <c r="L28" s="23">
-        <v>549899.56999999995</v>
+        <v>549899.56727395195</v>
       </c>
       <c r="N28" s="21">
-        <v>6.0202861999999998E-3</v>
+        <v>0</v>
       </c>
       <c r="O28" s="22">
         <v>0</v>
       </c>
       <c r="P28" s="23">
-        <v>6.1543062000000003E-2</v>
+        <v>0</v>
       </c>
       <c r="R28">
-        <v>6.0202861999999996E-2</v>
+        <v>0</v>
       </c>
       <c r="S28">
         <v>0</v>
       </c>
       <c r="T28">
-        <v>0.30771531000000002</v>
+        <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:20" x14ac:dyDescent="0.35">
@@ -1914,17 +3116,17 @@
       </c>
       <c r="N32">
         <f t="array" ref="N32:P36">J19:L19+MMULT(N46:R50,N24:P28)</f>
-        <v>1.7706724E-2</v>
+        <v>0</v>
       </c>
       <c r="O32">
-        <v>0</v>
+        <v>8.552347805392993E-2</v>
       </c>
       <c r="P32">
-        <v>2.8996700999999998</v>
+        <v>0.28996700913242007</v>
       </c>
       <c r="R32">
         <f t="array" ref="R32:T36">MMULT(J24:L28,_xlfn.MUNIT(3)*J15:L15)</f>
-        <v>1085.7763</v>
+        <v>0</v>
       </c>
       <c r="S32">
         <v>0</v>
@@ -1947,22 +3149,22 @@
         <v>0</v>
       </c>
       <c r="N33">
-        <v>2.1248068799999999E-2</v>
+        <v>0</v>
       </c>
       <c r="O33">
-        <v>0</v>
+        <v>8.552347805392993E-2</v>
       </c>
       <c r="P33">
-        <v>2.9576635019999999</v>
+        <v>0.29576634931506846</v>
       </c>
       <c r="R33">
-        <v>1302.9315999999999</v>
+        <v>0</v>
       </c>
       <c r="S33">
         <v>0</v>
       </c>
       <c r="T33">
-        <v>518182.64</v>
+        <v>518182.64399999997</v>
       </c>
     </row>
     <row r="34" spans="1:20" x14ac:dyDescent="0.35">
@@ -1979,22 +3181,22 @@
         <v>0</v>
       </c>
       <c r="N34">
-        <v>2.5497682599999998E-2</v>
+        <v>0</v>
       </c>
       <c r="O34">
-        <v>0</v>
+        <v>8.552347805392993E-2</v>
       </c>
       <c r="P34">
-        <v>3.0168167719999999</v>
+        <v>0.31386961602394514</v>
       </c>
       <c r="R34">
-        <v>1563.5178999999998</v>
+        <v>0</v>
       </c>
       <c r="S34">
         <v>0</v>
       </c>
       <c r="T34">
-        <v>528546.30000000005</v>
+        <v>528546.29688000004</v>
       </c>
     </row>
     <row r="35" spans="1:20" x14ac:dyDescent="0.35">
@@ -2011,22 +3213,22 @@
         <v>0</v>
       </c>
       <c r="N35">
-        <v>3.0632632599999998E-2</v>
+        <v>0</v>
       </c>
       <c r="O35">
-        <v>0</v>
+        <v>8.552347805392993E-2</v>
       </c>
       <c r="P35">
-        <v>3.077153107</v>
+        <v>0.31386961602394514</v>
       </c>
       <c r="R35">
-        <v>1878.3931000000002</v>
+        <v>0</v>
       </c>
       <c r="S35">
         <v>0</v>
       </c>
       <c r="T35">
-        <v>539117.22</v>
+        <v>539117.22281760001</v>
       </c>
     </row>
     <row r="36" spans="1:20" x14ac:dyDescent="0.35">
@@ -2043,22 +3245,22 @@
         <v>0</v>
       </c>
       <c r="N36">
-        <v>3.6652918799999996E-2</v>
+        <v>0</v>
       </c>
       <c r="O36">
-        <v>0</v>
+        <v>8.552347805392993E-2</v>
       </c>
       <c r="P36">
-        <v>3.1386961690000001</v>
+        <v>0.31386961602394514</v>
       </c>
       <c r="R36">
-        <v>2247.5569999999998</v>
+        <v>0</v>
       </c>
       <c r="S36">
         <v>0</v>
       </c>
       <c r="T36">
-        <v>549899.56999999995</v>
+        <v>549899.56727395195</v>
       </c>
     </row>
     <row r="38" spans="1:20" x14ac:dyDescent="0.35">
@@ -2072,13 +3274,13 @@
       </c>
       <c r="J39">
         <f t="array" ref="J39:L43">N32:P36*J18:L18*8760</f>
-        <v>108.57763156799999</v>
+        <v>0</v>
       </c>
       <c r="K39">
-        <v>0</v>
+        <v>224.75570032572784</v>
       </c>
       <c r="L39">
-        <v>508022.20151999994</v>
+        <v>508022.2</v>
       </c>
     </row>
     <row r="40" spans="1:20" x14ac:dyDescent="0.35">
@@ -2086,13 +3288,13 @@
         <v>25</v>
       </c>
       <c r="J40">
-        <v>130.29315788159997</v>
+        <v>0</v>
       </c>
       <c r="K40">
-        <v>0</v>
+        <v>224.75570032572784</v>
       </c>
       <c r="L40">
-        <v>518182.64555039996</v>
+        <v>518182.64399999991</v>
       </c>
     </row>
     <row r="41" spans="1:20" x14ac:dyDescent="0.35">
@@ -2100,13 +3302,13 @@
         <v>26</v>
       </c>
       <c r="J41">
-        <v>156.35178970319998</v>
+        <v>0</v>
       </c>
       <c r="K41">
-        <v>0</v>
+        <v>224.75570032572784</v>
       </c>
       <c r="L41">
-        <v>528546.29845440004</v>
+        <v>549899.56727395183</v>
       </c>
     </row>
     <row r="42" spans="1:20" x14ac:dyDescent="0.35">
@@ -2114,13 +3316,13 @@
         <v>27</v>
       </c>
       <c r="J42">
-        <v>187.8393031032</v>
+        <v>0</v>
       </c>
       <c r="K42">
-        <v>0</v>
+        <v>224.75570032572784</v>
       </c>
       <c r="L42">
-        <v>539117.22434640001</v>
+        <v>549899.56727395183</v>
       </c>
     </row>
     <row r="43" spans="1:20" x14ac:dyDescent="0.35">
@@ -2128,13 +3330,13 @@
         <v>28</v>
       </c>
       <c r="J43">
-        <v>224.75569808159997</v>
+        <v>0</v>
       </c>
       <c r="K43">
-        <v>0</v>
+        <v>224.75570032572784</v>
       </c>
       <c r="L43">
-        <v>549899.56880879996</v>
+        <v>549899.56727395183</v>
       </c>
     </row>
     <row r="45" spans="1:20" x14ac:dyDescent="0.35">
@@ -2243,8 +3445,8 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -6448,11 +7650,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93A526CD-DE21-40CC-88A4-8C9263AC5352}">
   <dimension ref="A1:AW52"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="5" ySplit="5" topLeftCell="F6" activePane="bottomRight" state="frozen"/>
+    <sheetView showGridLines="0" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane xSplit="5" ySplit="5" topLeftCell="F14" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="U7" sqref="U7:U8"/>
+      <selection pane="bottomRight" activeCell="R22" sqref="R22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>